<commit_message>
Added different survival functions for further investigation
</commit_message>
<xml_diff>
--- a/TempSuitability_CSharp/test_temp_conversion.xlsx
+++ b/TempSuitability_CSharp/test_temp_conversion.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>day</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>maxtemp_k</t>
+  </si>
+  <si>
+    <t>maxtemp_c_bug</t>
   </si>
 </sst>
 </file>
@@ -449,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P102"/>
+  <dimension ref="A1:Q102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23:J24"/>
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -462,11 +465,11 @@
     <col min="4" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="9.140625" style="3"/>
     <col min="8" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="9.140625" style="3"/>
-    <col min="11" max="11" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.140625" style="3"/>
+    <col min="12" max="12" width="12" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -498,16 +501,19 @@
         <v>10</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>5</v>
       </c>
-      <c r="P1">
+      <c r="Q1">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -537,7 +543,7 @@
         <v>-0.10430208973957018</v>
       </c>
       <c r="I2" s="1">
-        <f>24 - (24 / PI()) * ACOS(SIN(0.8333*PI()/180)+SIN($P$1*PI()/180)*SIN(H2)/(COS($P$1 *PI()/180)*COS(H2)))</f>
+        <f>24 - (24 / PI()) * ACOS(SIN(0.8333*PI()/180)+SIN($Q$1*PI()/180)*SIN(H2)/(COS($Q$1 *PI()/180)*COS(H2)))</f>
         <v>11.787971159891447</v>
       </c>
       <c r="J2" s="3">
@@ -545,11 +551,15 @@
         <v>22.040789994574766</v>
       </c>
       <c r="K2" s="3">
+        <f>18.148887+B2*0.949445+((B2-B2)*-0.541052)+(I2*-0.86562)</f>
+        <v>33.608481754574768</v>
+      </c>
+      <c r="L2" s="3">
         <f>(18.148887+D2*0.949445+((D2-E2)*-0.541052)+(I2*-0.86562))-273.14</f>
         <v>8.2321972945747461</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -579,7 +589,7 @@
         <v>-4.9710009879434795E-2</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3:I66" si="4">24 - (24 / PI()) * ACOS(SIN(0.8333*PI()/180)+SIN($P$1*PI()/180)*SIN(H3)/(COS($P$1 *PI()/180)*COS(H3)))</f>
+        <f t="shared" ref="I3:I66" si="4">24 - (24 / PI()) * ACOS(SIN(0.8333*PI()/180)+SIN($Q$1*PI()/180)*SIN(H3)/(COS($Q$1 *PI()/180)*COS(H3)))</f>
         <v>11.957544439080975</v>
       </c>
       <c r="J3" s="3">
@@ -587,11 +597,15 @@
         <v>25.81877544271433</v>
       </c>
       <c r="K3" s="3">
-        <f t="shared" ref="K3:K66" si="6">(18.148887+D3*0.949445+((D3-E3)*-0.541052)+(I3*-0.86562))-273.14</f>
+        <f t="shared" ref="K3:K66" si="6">18.148887+B3*0.949445+((B3-B3)*-0.541052)+(I3*-0.86562)</f>
+        <v>37.202510171976726</v>
+      </c>
+      <c r="L3" s="3">
+        <f t="shared" ref="L3:L66" si="7">(18.148887+D3*0.949445+((D3-E3)*-0.541052)+(I3*-0.86562))-273.14</f>
         <v>12.010182742714335</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -630,10 +644,14 @@
       </c>
       <c r="K4" s="3">
         <f t="shared" si="6"/>
+        <v>39.922314647076774</v>
+      </c>
+      <c r="L4" s="3">
+        <f t="shared" si="7"/>
         <v>11.894876523285973</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -672,10 +690,14 @@
       </c>
       <c r="K5" s="3">
         <f t="shared" si="6"/>
+        <v>44.01007515672913</v>
+      </c>
+      <c r="L5" s="3">
+        <f t="shared" si="7"/>
         <v>17.822214698621508</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -714,10 +736,14 @@
       </c>
       <c r="K6" s="3">
         <f t="shared" si="6"/>
+        <v>45.517549341187539</v>
+      </c>
+      <c r="L6" s="3">
+        <f t="shared" si="7"/>
         <v>19.697602241187553</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -756,10 +782,14 @@
       </c>
       <c r="K7" s="3">
         <f t="shared" si="6"/>
+        <v>44.788082243801675</v>
+      </c>
+      <c r="L7" s="3">
+        <f t="shared" si="7"/>
         <v>17.106916263801679</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -798,10 +828,14 @@
       </c>
       <c r="K8" s="3">
         <f t="shared" si="6"/>
+        <v>45.526289280834725</v>
+      </c>
+      <c r="L8" s="3">
+        <f t="shared" si="7"/>
         <v>18.180576677043916</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -840,10 +874,14 @@
       </c>
       <c r="K9" s="3">
         <f t="shared" si="6"/>
+        <v>46.025271618428476</v>
+      </c>
+      <c r="L9" s="3">
+        <f t="shared" si="7"/>
         <v>18.939264082848069</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -882,10 +920,14 @@
       </c>
       <c r="K10" s="3">
         <f t="shared" si="6"/>
+        <v>46.534344569132401</v>
+      </c>
+      <c r="L10" s="3">
+        <f t="shared" si="7"/>
         <v>18.853179887657234</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -924,10 +966,14 @@
       </c>
       <c r="K11" s="3">
         <f t="shared" si="6"/>
+        <v>47.948785389640953</v>
+      </c>
+      <c r="L11" s="3">
+        <f t="shared" si="7"/>
         <v>21.695996689640936</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -966,10 +1012,14 @@
       </c>
       <c r="K12" s="3">
         <f t="shared" si="6"/>
+        <v>47.897985566687325</v>
+      </c>
+      <c r="L12" s="3">
+        <f t="shared" si="7"/>
         <v>21.623556463948489</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1008,10 +1058,14 @@
       </c>
       <c r="K13" s="3">
         <f t="shared" si="6"/>
+        <v>50.866337830391586</v>
+      </c>
+      <c r="L13" s="3">
+        <f t="shared" si="7"/>
         <v>23.076962694811129</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1050,10 +1104,14 @@
       </c>
       <c r="K14" s="3">
         <f t="shared" si="6"/>
+        <v>49.431865616668894</v>
+      </c>
+      <c r="L14" s="3">
+        <f t="shared" si="7"/>
         <v>22.32421475666888</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1092,10 +1150,14 @@
       </c>
       <c r="K15" s="3">
         <f t="shared" si="6"/>
+        <v>46.653798323128882</v>
+      </c>
+      <c r="L15" s="3">
+        <f t="shared" si="7"/>
         <v>20.325263912179707</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1134,10 +1196,14 @@
       </c>
       <c r="K16" s="3">
         <f t="shared" si="6"/>
+        <v>47.755151320057188</v>
+      </c>
+      <c r="L16" s="3">
+        <f t="shared" si="7"/>
         <v>20.712428377318361</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1176,10 +1242,14 @@
       </c>
       <c r="K17" s="3">
         <f t="shared" si="6"/>
+        <v>49.564705031774167</v>
+      </c>
+      <c r="L17" s="3">
+        <f t="shared" si="7"/>
         <v>22.294739653878139</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1218,10 +1288,14 @@
       </c>
       <c r="K18" s="3">
         <f t="shared" si="6"/>
+        <v>49.081018389298876</v>
+      </c>
+      <c r="L18" s="3">
+        <f t="shared" si="7"/>
         <v>22.655094888875681</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1260,10 +1334,14 @@
       </c>
       <c r="K19" s="3">
         <f t="shared" si="6"/>
+        <v>47.517268885553392</v>
+      </c>
+      <c r="L19" s="3">
+        <f t="shared" si="7"/>
         <v>21.480900985553433</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1302,10 +1380,14 @@
       </c>
       <c r="K20" s="3">
         <f t="shared" si="6"/>
+        <v>47.624103236206118</v>
+      </c>
+      <c r="L20" s="3">
+        <f t="shared" si="7"/>
         <v>22.096324216206142</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1344,10 +1426,14 @@
       </c>
       <c r="K21" s="3">
         <f t="shared" si="6"/>
+        <v>48.335137515662993</v>
+      </c>
+      <c r="L21" s="3">
+        <f t="shared" si="7"/>
         <v>21.909212879030576</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1386,10 +1472,14 @@
       </c>
       <c r="K22" s="3">
         <f t="shared" si="6"/>
+        <v>46.324330697289518</v>
+      </c>
+      <c r="L22" s="3">
+        <f t="shared" si="7"/>
         <v>22.744340284024759</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1428,10 +1518,14 @@
       </c>
       <c r="K23" s="3">
         <f t="shared" si="6"/>
+        <v>50.38080534788368</v>
+      </c>
+      <c r="L23" s="3">
+        <f t="shared" si="7"/>
         <v>23.175766859250075</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1470,10 +1564,14 @@
       </c>
       <c r="K24" s="3">
         <f t="shared" si="6"/>
+        <v>47.741628171526372</v>
+      </c>
+      <c r="L24" s="3">
+        <f t="shared" si="7"/>
         <v>21.553765711526353</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1512,10 +1610,14 @@
       </c>
       <c r="K25" s="3">
         <f t="shared" si="6"/>
+        <v>50.823505368640333</v>
+      </c>
+      <c r="L25" s="3">
+        <f t="shared" si="7"/>
         <v>23.120698877691098</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1554,10 +1656,14 @@
       </c>
       <c r="K26" s="3">
         <f t="shared" si="6"/>
+        <v>48.668151533067828</v>
+      </c>
+      <c r="L26" s="3">
+        <f t="shared" si="7"/>
         <v>21.928416682330294</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1596,10 +1702,14 @@
       </c>
       <c r="K27" s="3">
         <f t="shared" si="6"/>
+        <v>46.363112906219278</v>
+      </c>
+      <c r="L27" s="3">
+        <f t="shared" si="7"/>
         <v>19.83979977527008</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1638,10 +1748,14 @@
       </c>
       <c r="K28" s="3">
         <f t="shared" si="6"/>
+        <v>46.660435692433808</v>
+      </c>
+      <c r="L28" s="3">
+        <f t="shared" si="7"/>
         <v>20.569964269694992</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1680,10 +1794,14 @@
       </c>
       <c r="K29" s="3">
         <f t="shared" si="6"/>
+        <v>48.514359722092003</v>
+      </c>
+      <c r="L29" s="3">
+        <f t="shared" si="7"/>
         <v>21.298499111354431</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1722,10 +1840,14 @@
       </c>
       <c r="K30" s="3">
         <f t="shared" si="6"/>
+        <v>43.606207588853955</v>
+      </c>
+      <c r="L30" s="3">
+        <f t="shared" si="7"/>
         <v>18.446343928853935</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1764,10 +1886,14 @@
       </c>
       <c r="K31" s="3">
         <f t="shared" si="6"/>
+        <v>41.998261532814304</v>
+      </c>
+      <c r="L31" s="3">
+        <f t="shared" si="7"/>
         <v>14.598442592814308</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1806,10 +1932,14 @@
       </c>
       <c r="K32" s="3">
         <f t="shared" si="6"/>
+        <v>40.232271773231268</v>
+      </c>
+      <c r="L32" s="3">
+        <f t="shared" si="7"/>
         <v>13.4384310732313</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1848,10 +1978,14 @@
       </c>
       <c r="K33" s="3">
         <f t="shared" si="6"/>
+        <v>38.362414963261195</v>
+      </c>
+      <c r="L33" s="3">
+        <f t="shared" si="7"/>
         <v>12.12044730326113</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1890,10 +2024,14 @@
       </c>
       <c r="K34" s="3">
         <f t="shared" si="6"/>
+        <v>39.043816252769631</v>
+      </c>
+      <c r="L34" s="3">
+        <f t="shared" si="7"/>
         <v>12.390649072769634</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1932,10 +2070,14 @@
       </c>
       <c r="K35" s="3">
         <f t="shared" si="6"/>
+        <v>33.271996198006427</v>
+      </c>
+      <c r="L35" s="3">
+        <f t="shared" si="7"/>
         <v>8.956173658006378</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1974,10 +2116,14 @@
       </c>
       <c r="K36" s="3">
         <f t="shared" si="6"/>
+        <v>31.543923824468184</v>
+      </c>
+      <c r="L36" s="3">
+        <f t="shared" si="7"/>
         <v>7.5635535244682046</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2016,10 +2162,14 @@
       </c>
       <c r="K37" s="3">
         <f t="shared" si="6"/>
+        <v>28.083354422295894</v>
+      </c>
+      <c r="L37" s="3">
+        <f t="shared" si="7"/>
         <v>5.0444146022959444</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2058,10 +2208,14 @@
       </c>
       <c r="K38" s="3">
         <f t="shared" si="6"/>
+        <v>33.293379203649536</v>
+      </c>
+      <c r="L38" s="3">
+        <f t="shared" si="7"/>
         <v>7.3760426733127247</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2100,10 +2254,14 @@
       </c>
       <c r="K39" s="3">
         <f t="shared" si="6"/>
+        <v>34.506854491135137</v>
+      </c>
+      <c r="L39" s="3">
+        <f t="shared" si="7"/>
         <v>7.799581407767505</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2142,10 +2300,14 @@
       </c>
       <c r="K40" s="3">
         <f t="shared" si="6"/>
+        <v>28.147948114100881</v>
+      </c>
+      <c r="L40" s="3">
+        <f t="shared" si="7"/>
         <v>4.3839985654061593</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2184,10 +2346,14 @@
       </c>
       <c r="K41" s="3">
         <f t="shared" si="6"/>
+        <v>31.765479346765318</v>
+      </c>
+      <c r="L41" s="3">
+        <f t="shared" si="7"/>
         <v>7.1683097667653328</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2226,10 +2392,14 @@
       </c>
       <c r="K42" s="3">
         <f t="shared" si="6"/>
+        <v>27.895900779233806</v>
+      </c>
+      <c r="L42" s="3">
+        <f t="shared" si="7"/>
         <v>4.0778460792338365</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2268,10 +2438,14 @@
       </c>
       <c r="K43" s="3">
         <f t="shared" si="6"/>
+        <v>30.97421649935869</v>
+      </c>
+      <c r="L43" s="3">
+        <f t="shared" si="7"/>
         <v>5.9658473993586654</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2310,10 +2484,14 @@
       </c>
       <c r="K44" s="3">
         <f t="shared" si="6"/>
+        <v>27.408247087056932</v>
+      </c>
+      <c r="L44" s="3">
+        <f t="shared" si="7"/>
         <v>2.5838356670569169</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2352,10 +2530,14 @@
       </c>
       <c r="K45" s="3">
         <f t="shared" si="6"/>
+        <v>28.842028504478399</v>
+      </c>
+      <c r="L45" s="3">
+        <f t="shared" si="7"/>
         <v>4.3530693244783834</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2394,10 +2576,14 @@
       </c>
       <c r="K46" s="3">
         <f t="shared" si="6"/>
+        <v>34.063760054745899</v>
+      </c>
+      <c r="L46" s="3">
+        <f t="shared" si="7"/>
         <v>7.4646975336938794</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2436,10 +2622,14 @@
       </c>
       <c r="K47" s="3">
         <f t="shared" si="6"/>
+        <v>37.58862693779183</v>
+      </c>
+      <c r="L47" s="3">
+        <f t="shared" si="7"/>
         <v>11.097775357791818</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2478,10 +2668,14 @@
       </c>
       <c r="K48" s="3">
         <f t="shared" si="6"/>
+        <v>38.602559701184262</v>
+      </c>
+      <c r="L48" s="3">
+        <f t="shared" si="7"/>
         <v>12.512088170235074</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -2520,10 +2714,14 @@
       </c>
       <c r="K49" s="3">
         <f t="shared" si="6"/>
+        <v>43.202998679252218</v>
+      </c>
+      <c r="L49" s="3">
+        <f t="shared" si="7"/>
         <v>14.861750828303002</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2562,10 +2760,14 @@
       </c>
       <c r="K50" s="3">
         <f t="shared" si="6"/>
+        <v>46.492476040911271</v>
+      </c>
+      <c r="L50" s="3">
+        <f t="shared" si="7"/>
         <v>17.123228145542498</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -2604,10 +2806,14 @@
       </c>
       <c r="K51" s="3">
         <f t="shared" si="6"/>
+        <v>38.446330400008634</v>
+      </c>
+      <c r="L51" s="3">
+        <f t="shared" si="7"/>
         <v>11.739058020008599</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2646,10 +2852,14 @@
       </c>
       <c r="K52" s="3">
         <f t="shared" si="6"/>
+        <v>42.764156087797041</v>
+      </c>
+      <c r="L52" s="3">
+        <f t="shared" si="7"/>
         <v>15.472549549689461</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2688,10 +2898,14 @@
       </c>
       <c r="K53" s="3">
         <f t="shared" si="6"/>
+        <v>44.807071143801672</v>
+      </c>
+      <c r="L53" s="3">
+        <f t="shared" si="7"/>
         <v>19.160261224853627</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2730,10 +2944,14 @@
       </c>
       <c r="K54" s="3">
         <f t="shared" si="6"/>
+        <v>44.671790774669226</v>
+      </c>
+      <c r="L54" s="3">
+        <f t="shared" si="7"/>
         <v>19.176474874669225</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2772,10 +2990,14 @@
       </c>
       <c r="K55" s="3">
         <f t="shared" si="6"/>
+        <v>49.310350463927975</v>
+      </c>
+      <c r="L55" s="3">
+        <f t="shared" si="7"/>
         <v>22.408301095294405</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2814,10 +3036,14 @@
       </c>
       <c r="K56" s="3">
         <f t="shared" si="6"/>
+        <v>44.882312547800396</v>
+      </c>
+      <c r="L56" s="3">
+        <f t="shared" si="7"/>
         <v>18.759376327800453</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2856,10 +3082,14 @@
       </c>
       <c r="K57" s="3">
         <f t="shared" si="6"/>
+        <v>49.942619889640959</v>
+      </c>
+      <c r="L57" s="3">
+        <f t="shared" si="7"/>
         <v>20.735687864798138</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2898,10 +3128,14 @@
       </c>
       <c r="K58" s="3">
         <f t="shared" si="6"/>
+        <v>46.777640181853826</v>
+      </c>
+      <c r="L58" s="3">
+        <f t="shared" si="7"/>
         <v>21.747630841430578</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2940,10 +3174,14 @@
       </c>
       <c r="K59" s="3">
         <f t="shared" si="6"/>
+        <v>48.15092456072459</v>
+      </c>
+      <c r="L59" s="3">
+        <f t="shared" si="7"/>
         <v>22.590683989775414</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2982,10 +3220,14 @@
       </c>
       <c r="K60" s="3">
         <f t="shared" si="6"/>
+        <v>52.659978616668901</v>
+      </c>
+      <c r="L60" s="3">
+        <f t="shared" si="7"/>
         <v>24.264624591826077</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -3024,10 +3266,14 @@
       </c>
       <c r="K61" s="3">
         <f t="shared" si="6"/>
+        <v>56.749888098434191</v>
+      </c>
+      <c r="L61" s="3">
+        <f t="shared" si="7"/>
         <v>26.410168161808201</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -3066,10 +3312,14 @@
       </c>
       <c r="K62" s="3">
         <f t="shared" si="6"/>
+        <v>48.007617130664158</v>
+      </c>
+      <c r="L62" s="3">
+        <f t="shared" si="7"/>
         <v>22.425732910664181</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -3108,10 +3358,14 @@
       </c>
       <c r="K63" s="3">
         <f t="shared" si="6"/>
+        <v>49.365855117411883</v>
+      </c>
+      <c r="L63" s="3">
+        <f t="shared" si="7"/>
         <v>23.491802817411894</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -3150,10 +3404,14 @@
       </c>
       <c r="K64" s="3">
         <f t="shared" si="6"/>
+        <v>49.454136685553394</v>
+      </c>
+      <c r="L64" s="3">
+        <f t="shared" si="7"/>
         <v>23.742399985553391</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -3192,10 +3450,14 @@
       </c>
       <c r="K65" s="3">
         <f t="shared" si="6"/>
+        <v>48.079836836206105</v>
+      </c>
+      <c r="L65" s="3">
+        <f t="shared" si="7"/>
         <v>23.060646696206106</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -3234,10 +3496,14 @@
       </c>
       <c r="K66" s="3">
         <f t="shared" si="6"/>
+        <v>49.208624352161493</v>
+      </c>
+      <c r="L66" s="3">
+        <f t="shared" si="7"/>
         <v>23.940551753001955</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -3248,38 +3514,42 @@
         <v>22.09</v>
       </c>
       <c r="D67" s="1">
-        <f t="shared" ref="D67:D102" si="7">B67+273.14</f>
+        <f t="shared" ref="D67:D102" si="8">B67+273.14</f>
         <v>317.2699973</v>
       </c>
       <c r="E67" s="1">
-        <f t="shared" ref="E67:E102" si="8">C67+273.14</f>
+        <f t="shared" ref="E67:E102" si="9">C67+273.14</f>
         <v>295.22999999999996</v>
       </c>
       <c r="F67" s="1">
         <v>225</v>
       </c>
       <c r="G67" s="3">
-        <f t="shared" ref="G67:G102" si="9">0.209087+0.970841*C67</f>
+        <f t="shared" ref="G67:G102" si="10">0.209087+0.970841*C67</f>
         <v>21.65496469</v>
       </c>
       <c r="H67" s="1">
-        <f t="shared" ref="H67:H102" si="10">(ASIN(0.39795*COS(0.2163108+2*ATAN(0.9671396*TAN(0.0086*(F67-186))))))</f>
+        <f t="shared" ref="H67:H102" si="11">(ASIN(0.39795*COS(0.2163108+2*ATAN(0.9671396*TAN(0.0086*(F67-186))))))</f>
         <v>0.26057660212759171</v>
       </c>
       <c r="I67" s="1">
-        <f t="shared" ref="I67:I102" si="11">24 - (24 / PI()) * ACOS(SIN(0.8333*PI()/180)+SIN($P$1*PI()/180)*SIN(H67)/(COS($P$1 *PI()/180)*COS(H67)))</f>
+        <f t="shared" ref="I67:I102" si="12">24 - (24 / PI()) * ACOS(SIN(0.8333*PI()/180)+SIN($Q$1*PI()/180)*SIN(H67)/(COS($Q$1 *PI()/180)*COS(H67)))</f>
         <v>12.936436293238927</v>
       </c>
       <c r="J67" s="3">
-        <f t="shared" ref="J67:J102" si="12">18.148887+B67*0.949445+((B67-C67)*-0.541052)+(I67*-0.86562)</f>
+        <f t="shared" ref="J67:J102" si="13">18.148887+B67*0.949445+((B67-C67)*-0.541052)+(I67*-0.86562)</f>
         <v>36.92506968318542</v>
       </c>
       <c r="K67" s="3">
-        <f t="shared" ref="K67:K102" si="13">(18.148887+D67*0.949445+((D67-E67)*-0.541052)+(I67*-0.86562))-273.14</f>
+        <f t="shared" ref="K67:K102" si="14">18.148887+B67*0.949445+((B67-B67)*-0.541052)+(I67*-0.86562)</f>
+        <v>48.849854302345015</v>
+      </c>
+      <c r="L67" s="3">
+        <f t="shared" ref="L67:L102" si="15">(18.148887+D67*0.949445+((D67-E67)*-0.541052)+(I67*-0.86562))-273.14</f>
         <v>23.116476983185464</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -3290,38 +3560,42 @@
         <v>22.31</v>
       </c>
       <c r="D68" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>315.1099974</v>
       </c>
       <c r="E68" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>295.45</v>
       </c>
       <c r="F68" s="1">
         <v>233</v>
       </c>
       <c r="G68" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>21.868549709999996</v>
       </c>
       <c r="H68" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.21642200856137356</v>
       </c>
       <c r="I68" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>12.791138217569278</v>
       </c>
       <c r="J68" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>36.287745204285883</v>
       </c>
       <c r="K68" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>46.92482611755068</v>
+      </c>
+      <c r="L68" s="3">
+        <f t="shared" si="15"/>
         <v>22.479152504285878</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -3332,38 +3606,42 @@
         <v>20.29</v>
       </c>
       <c r="D69" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>318.12999789999998</v>
       </c>
       <c r="E69" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>293.43</v>
       </c>
       <c r="F69" s="1">
         <v>241</v>
       </c>
       <c r="G69" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>19.90745089</v>
       </c>
       <c r="H69" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.16861335767361324</v>
       </c>
       <c r="I69" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>12.637261013462755</v>
       </c>
       <c r="J69" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>36.561366413901069</v>
       </c>
       <c r="K69" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>49.925349677691869</v>
+      </c>
+      <c r="L69" s="3">
+        <f t="shared" si="15"/>
         <v>22.752773713901092</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -3374,38 +3652,42 @@
         <v>22.07</v>
       </c>
       <c r="D70" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>317.33</v>
       </c>
       <c r="E70" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>295.20999999999998</v>
       </c>
       <c r="F70" s="1">
         <v>249</v>
       </c>
       <c r="G70" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>21.63554787</v>
       </c>
       <c r="H70" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.11794260013308597</v>
       </c>
       <c r="I70" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>12.477144044695322</v>
       </c>
       <c r="J70" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>37.336325882030835</v>
       </c>
       <c r="K70" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>49.30439612203083</v>
+      </c>
+      <c r="L70" s="3">
+        <f t="shared" si="15"/>
         <v>23.527733182030829</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -3416,38 +3698,42 @@
         <v>21.01</v>
       </c>
       <c r="D71" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>315.49</v>
       </c>
       <c r="E71" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>294.14999999999998</v>
       </c>
       <c r="F71" s="1">
         <v>257</v>
       </c>
       <c r="G71" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>20.60645641</v>
       </c>
       <c r="H71" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>6.5211335925576056E-2</v>
       </c>
       <c r="I71" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>12.312752844125788</v>
       </c>
       <c r="J71" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>36.153667953067838</v>
       </c>
       <c r="K71" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>47.699717633067834</v>
+      </c>
+      <c r="L71" s="3">
+        <f t="shared" si="15"/>
         <v>22.345075253067876</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -3458,38 +3744,42 @@
         <v>20.550001099999999</v>
       </c>
       <c r="D72" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>315.37</v>
       </c>
       <c r="E72" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>293.69000109999996</v>
       </c>
       <c r="F72" s="1">
         <v>265</v>
       </c>
       <c r="G72" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>20.159870617925097</v>
       </c>
       <c r="H72" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.1232728280784856E-2</v>
       </c>
       <c r="I72" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>12.145783242520066</v>
       </c>
       <c r="J72" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>36.000309694766976</v>
       </c>
       <c r="K72" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>47.730316459609774</v>
+      </c>
+      <c r="L72" s="3">
+        <f t="shared" si="15"/>
         <v>22.191716994766978</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -3500,38 +3790,42 @@
         <v>19.95</v>
       </c>
       <c r="D73" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>315.07</v>
       </c>
       <c r="E73" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>293.08999999999997</v>
       </c>
       <c r="F73" s="1">
         <v>273</v>
       </c>
       <c r="G73" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>19.57736495</v>
       </c>
       <c r="H73" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-4.3162466293620916E-2</v>
       </c>
       <c r="I73" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11.977797548909104</v>
       </c>
       <c r="J73" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>35.698571775713305</v>
       </c>
       <c r="K73" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>47.590894735713306</v>
+      </c>
+      <c r="L73" s="3">
+        <f t="shared" si="15"/>
         <v>21.889979075713313</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -3542,38 +3836,42 @@
         <v>16.45</v>
       </c>
       <c r="D74" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>309.20999999999998</v>
       </c>
       <c r="E74" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>289.58999999999997</v>
       </c>
       <c r="F74" s="1">
         <v>281</v>
       </c>
       <c r="G74" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>16.17942145</v>
       </c>
       <c r="H74" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-9.7117837263074755E-2</v>
       </c>
       <c r="I74" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11.810379875589751</v>
       </c>
       <c r="J74" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>31.556626882091997</v>
       </c>
       <c r="K74" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>42.172067122091995</v>
+      </c>
+      <c r="L74" s="3">
+        <f t="shared" si="15"/>
         <v>17.748034182091999</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -3584,38 +3882,42 @@
         <v>14.39</v>
       </c>
       <c r="D75" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>309.78999769999996</v>
       </c>
       <c r="E75" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>287.52999999999997</v>
       </c>
       <c r="F75" s="1">
         <v>289</v>
       </c>
       <c r="G75" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>14.179488989999999</v>
       </c>
       <c r="H75" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.14974346051386658</v>
       </c>
       <c r="I75" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11.645301357577285</v>
       </c>
       <c r="J75" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>30.821822029550056</v>
       </c>
       <c r="K75" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>42.865638305130453</v>
+      </c>
+      <c r="L75" s="3">
+        <f t="shared" si="15"/>
         <v>17.013229329550029</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -3626,38 +3928,42 @@
         <v>11.85</v>
       </c>
       <c r="D76" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>303.64999999999998</v>
       </c>
       <c r="E76" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>284.99</v>
       </c>
       <c r="F76" s="1">
         <v>297</v>
       </c>
       <c r="G76" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11.713552849999999</v>
       </c>
       <c r="H76" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.20011073720370579</v>
       </c>
       <c r="I76" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11.48468498554297</v>
       </c>
       <c r="J76" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>27.079050612814292</v>
       </c>
       <c r="K76" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>37.175080932814296</v>
+      </c>
+      <c r="L76" s="3">
+        <f t="shared" si="15"/>
         <v>13.270457912814322</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -3668,38 +3974,42 @@
         <v>8.5700009999999995</v>
       </c>
       <c r="D77" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>302.39</v>
       </c>
       <c r="E77" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>281.71000099999998</v>
       </c>
       <c r="F77" s="1">
         <v>305</v>
       </c>
       <c r="G77" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8.5291953408409995</v>
       </c>
       <c r="H77" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.24725281472554392</v>
       </c>
       <c r="I77" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11.331153135057802</v>
       </c>
       <c r="J77" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>24.922725654283269</v>
       </c>
       <c r="K77" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>36.111680473231267</v>
+      </c>
+      <c r="L77" s="3">
+        <f t="shared" si="15"/>
         <v>11.114132954283264</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -3710,38 +4020,42 @@
         <v>11.6900005</v>
       </c>
       <c r="D78" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>308.84999999999997</v>
       </c>
       <c r="E78" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>284.83000049999998</v>
       </c>
       <c r="F78" s="1">
         <v>313</v>
       </c>
       <c r="G78" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11.558218775420499</v>
       </c>
       <c r="H78" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.29017383591281248</v>
       </c>
       <c r="I78" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11.187928983547977</v>
       </c>
       <c r="J78" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>29.373004093787202</v>
       </c>
       <c r="K78" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>42.369072863261202</v>
+      </c>
+      <c r="L78" s="3">
+        <f t="shared" si="15"/>
         <v>15.564411393787168</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -3752,38 +4066,42 @@
         <v>8.89</v>
       </c>
       <c r="D79" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>303.99</v>
       </c>
       <c r="E79" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>282.02999999999997</v>
       </c>
       <c r="F79" s="1">
         <v>321</v>
       </c>
       <c r="G79" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>8.8398634900000008</v>
       </c>
       <c r="H79" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.32787026913008305</v>
       </c>
       <c r="I79" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11.058848914339288</v>
       </c>
       <c r="J79" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>25.985002532769627</v>
       </c>
       <c r="K79" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>37.866504452769625</v>
+      </c>
+      <c r="L79" s="3">
+        <f t="shared" si="15"/>
         <v>12.17640983276965</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -3794,38 +4112,42 @@
         <v>6.79</v>
       </c>
       <c r="D80" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>300.99</v>
       </c>
       <c r="E80" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>279.93</v>
       </c>
       <c r="F80" s="1">
         <v>329</v>
       </c>
       <c r="G80" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.8010973899999998</v>
       </c>
       <c r="H80" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.3593667116871464</v>
       </c>
       <c r="I80" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>10.948234504740615</v>
       </c>
       <c r="J80" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>23.719364378006432</v>
       </c>
       <c r="K80" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>35.113919498006432</v>
+      </c>
+      <c r="L80" s="3">
+        <f t="shared" si="15"/>
         <v>9.9107716780064266</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -3836,38 +4158,42 @@
         <v>5.15</v>
       </c>
       <c r="D81" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>299.1100012</v>
       </c>
       <c r="E81" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>278.28999999999996</v>
       </c>
       <c r="F81" s="1">
         <v>337</v>
       </c>
       <c r="G81" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.2089181500000006</v>
       </c>
       <c r="H81" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.38376629466869333</v>
       </c>
       <c r="I81" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>10.860582733222214</v>
       </c>
       <c r="J81" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>22.140133874539789</v>
       </c>
       <c r="K81" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>33.404837163802185</v>
+      </c>
+      <c r="L81" s="3">
+        <f t="shared" si="15"/>
         <v>8.3315411745397796</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -3878,38 +4204,42 @@
         <v>5.0299997300000001</v>
       </c>
       <c r="D82" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>299.37</v>
       </c>
       <c r="E82" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>278.16999972999997</v>
       </c>
       <c r="F82" s="1">
         <v>345</v>
       </c>
       <c r="G82" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.0924169678729303</v>
       </c>
       <c r="H82" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.40031197030199439</v>
       </c>
       <c r="I82" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>10.800074545070707</v>
       </c>
       <c r="J82" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>22.233766276211849</v>
       </c>
       <c r="K82" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>33.704068822295895</v>
+      </c>
+      <c r="L82" s="3">
+        <f t="shared" si="15"/>
         <v>8.4251735762118756</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -3920,38 +4250,42 @@
         <v>6.0699996900000004</v>
       </c>
       <c r="D83" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>300.03000129999998</v>
       </c>
       <c r="E83" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>279.20999968999996</v>
       </c>
       <c r="F83" s="1">
         <v>353</v>
       </c>
       <c r="G83" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.1020915690392901</v>
       </c>
       <c r="H83" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.40845024822266707</v>
       </c>
       <c r="I83" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>10.769974638236711</v>
       </c>
       <c r="J83" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>23.092055326834313</v>
       </c>
       <c r="K83" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>34.356758837928034</v>
+      </c>
+      <c r="L83" s="3">
+        <f t="shared" si="15"/>
         <v>9.2834626268343072</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -3962,38 +4296,42 @@
         <v>5.29</v>
       </c>
       <c r="D84" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>292.70999999999998</v>
       </c>
       <c r="E84" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>278.43</v>
       </c>
       <c r="F84" s="1">
         <v>361</v>
       </c>
       <c r="G84" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.3448358899999997</v>
       </c>
       <c r="H84" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.40788522968924845</v>
       </c>
       <c r="I84" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>10.772071813560649</v>
       </c>
       <c r="J84" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>19.67878228674563</v>
       </c>
       <c r="K84" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>27.405004846745634</v>
+      </c>
+      <c r="L84" s="3">
+        <f t="shared" si="15"/>
         <v>5.8701895867456528</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -4004,38 +4342,42 @@
         <v>1.89</v>
       </c>
       <c r="D85" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>292.69000109999996</v>
       </c>
       <c r="E85" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>275.02999999999997</v>
       </c>
       <c r="F85" s="1">
         <v>1</v>
       </c>
       <c r="G85" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2.0439764899999999</v>
       </c>
       <c r="H85" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.40270065067443078</v>
       </c>
       <c r="I85" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>10.791263528914676</v>
       </c>
       <c r="J85" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17.814425343333173</v>
       </c>
       <c r="K85" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>27.369404258490373</v>
+      </c>
+      <c r="L85" s="3">
+        <f t="shared" si="15"/>
         <v>4.0058326433331217</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -4046,38 +4388,42 @@
         <v>0.54999995199999996</v>
       </c>
       <c r="D86" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>290.49</v>
       </c>
       <c r="E86" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>273.68999995199999</v>
       </c>
       <c r="F86" s="1">
         <v>9</v>
       </c>
       <c r="G86" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.74304950339963194</v>
       </c>
       <c r="H86" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.38779367890004862</v>
       </c>
       <c r="I86" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>10.845937019979537</v>
       </c>
       <c r="J86" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>16.143624120794819</v>
       </c>
       <c r="K86" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>25.233297746765317</v>
+      </c>
+      <c r="L86" s="3">
+        <f t="shared" si="15"/>
         <v>2.3350314207948486</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -4088,38 +4434,42 @@
         <v>1.53</v>
       </c>
       <c r="D87" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>293.83</v>
       </c>
       <c r="E87" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>274.66999999999996</v>
       </c>
       <c r="F87" s="1">
         <v>17</v>
       </c>
       <c r="G87" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.6944737299999999</v>
       </c>
       <c r="H87" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.36479720208847966</v>
       </c>
       <c r="I87" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>10.928881692620545</v>
       </c>
       <c r="J87" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17.96608915923381</v>
       </c>
       <c r="K87" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>28.332645479233811</v>
+      </c>
+      <c r="L87" s="3">
+        <f t="shared" si="15"/>
         <v>4.1574964592337551</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -4130,38 +4480,42 @@
         <v>2.6899998200000002</v>
       </c>
       <c r="D88" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>292.33</v>
       </c>
       <c r="E88" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>275.82999982000001</v>
       </c>
       <c r="F88" s="1">
         <v>25</v>
       </c>
       <c r="G88" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>2.8206491152486199</v>
       </c>
       <c r="H88" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.33440364963266606</v>
       </c>
       <c r="I88" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11.036123415172149</v>
       </c>
       <c r="J88" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17.888289301969323</v>
       </c>
       <c r="K88" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>26.815647399358681</v>
+      </c>
+      <c r="L88" s="3">
+        <f t="shared" si="15"/>
         <v>4.0796966019693173</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -4172,38 +4526,42 @@
         <v>1.75</v>
       </c>
       <c r="D89" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>291.81</v>
       </c>
       <c r="E89" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>274.89</v>
       </c>
       <c r="F89" s="1">
         <v>33</v>
       </c>
       <c r="G89" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.9080587499999999</v>
       </c>
       <c r="H89" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.29747452898734572</v>
       </c>
       <c r="I89" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11.163187961164326</v>
       </c>
       <c r="J89" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>17.057346547056934</v>
       </c>
       <c r="K89" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>26.211946387056937</v>
+      </c>
+      <c r="L89" s="3">
+        <f t="shared" si="15"/>
         <v>3.2487538470569461</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -4214,38 +4572,42 @@
         <v>4.0099997500000004</v>
       </c>
       <c r="D90" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>297.83</v>
       </c>
       <c r="E90" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>277.14999975000001</v>
       </c>
       <c r="F90" s="1">
         <v>41</v>
       </c>
       <c r="G90" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4.1021591672897504</v>
       </c>
       <c r="H90" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.2549778242878894</v>
       </c>
       <c r="I90" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11.305638901043871</v>
       </c>
       <c r="J90" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>20.615341409215407</v>
       </c>
       <c r="K90" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>31.804296904478406</v>
+      </c>
+      <c r="L90" s="3">
+        <f t="shared" si="15"/>
         <v>6.8067487092154124</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -4256,38 +4618,42 @@
         <v>3.09</v>
       </c>
       <c r="D91" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>301.43</v>
       </c>
       <c r="E91" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>276.22999999999996</v>
       </c>
       <c r="F91" s="1">
         <v>49</v>
       </c>
       <c r="G91" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3.2089856899999996</v>
       </c>
       <c r="H91" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.20793317693271399</v>
       </c>
       <c r="I91" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11.459446806565344</v>
       </c>
       <c r="J91" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>21.454649305300904</v>
       </c>
       <c r="K91" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>35.089159705300901</v>
+      </c>
+      <c r="L91" s="3">
+        <f t="shared" si="15"/>
         <v>7.6460566053009416</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -4298,38 +4664,42 @@
         <v>5.0099997500000004</v>
       </c>
       <c r="D92" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>300.45</v>
       </c>
       <c r="E92" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>278.14999975000001</v>
       </c>
       <c r="F92" s="1">
         <v>57</v>
       </c>
       <c r="G92" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5.0730001672897505</v>
       </c>
       <c r="H92" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.15737033640379361</v>
       </c>
       <c r="I92" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11.621168887280984</v>
       </c>
       <c r="J92" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>21.95325400252883</v>
       </c>
       <c r="K92" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>34.018713737791828</v>
+      </c>
+      <c r="L92" s="3">
+        <f t="shared" si="15"/>
         <v>8.1446613025288457</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -4340,38 +4710,42 @@
         <v>9.5300010000000004</v>
       </c>
       <c r="D93" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>305.70999999999998</v>
       </c>
       <c r="E93" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>282.67000100000001</v>
       </c>
       <c r="F93" s="1">
         <v>65</v>
       </c>
       <c r="G93" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>9.4612027008409996</v>
       </c>
       <c r="H93" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.10430208973957018</v>
       </c>
       <c r="I93" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11.787971159891447</v>
       </c>
       <c r="J93" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>26.402569515626766</v>
       </c>
       <c r="K93" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>38.868407054574767</v>
+      </c>
+      <c r="L93" s="3">
+        <f t="shared" si="15"/>
         <v>12.593976815626775</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -4382,38 +4756,42 @@
         <v>11.51</v>
       </c>
       <c r="D94" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>304.31</v>
       </c>
       <c r="E94" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>284.64999999999998</v>
       </c>
       <c r="F94" s="1">
         <v>73</v>
       </c>
       <c r="G94" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11.383466909999999</v>
       </c>
       <c r="H94" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-4.9710009879434795E-2</v>
       </c>
       <c r="I94" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>11.957544439080975</v>
       </c>
       <c r="J94" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>26.75531571264273</v>
       </c>
       <c r="K94" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>37.392398032642731</v>
+      </c>
+      <c r="L94" s="3">
+        <f t="shared" si="15"/>
         <v>12.946723012642735</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -4424,38 +4802,42 @@
         <v>15.43</v>
       </c>
       <c r="D95" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>310.28999769999996</v>
       </c>
       <c r="E95" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>288.57</v>
       </c>
       <c r="F95" s="1">
         <v>81</v>
       </c>
       <c r="G95" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>15.189163629999999</v>
       </c>
       <c r="H95" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5.4599951886842163E-3</v>
       </c>
       <c r="I95" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>12.127961356124773</v>
       </c>
       <c r="J95" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>31.170912461607372</v>
       </c>
       <c r="K95" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>42.922560657187773</v>
+      </c>
+      <c r="L95" s="3">
+        <f t="shared" si="15"/>
         <v>17.362319761607353</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -4466,38 +4848,42 @@
         <v>11.910000800000001</v>
       </c>
       <c r="D96" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>304.22999999999996</v>
       </c>
       <c r="E96" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>285.05000079999996</v>
       </c>
       <c r="F96" s="1">
         <v>89</v>
       </c>
       <c r="G96" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>11.7718040866728</v>
       </c>
       <c r="H96" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>6.0295649556938738E-2</v>
       </c>
       <c r="I96" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>12.297508317727599</v>
       </c>
       <c r="J96" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>26.644785972850233</v>
       </c>
       <c r="K96" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>37.022162900008638</v>
+      </c>
+      <c r="L96" s="3">
+        <f t="shared" si="15"/>
         <v>12.83619327285021</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -4508,38 +4894,42 @@
         <v>16.970001199999999</v>
       </c>
       <c r="D97" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>312.1099974</v>
       </c>
       <c r="E97" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>290.1100012</v>
       </c>
       <c r="F97" s="1">
         <v>97</v>
       </c>
       <c r="G97" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>16.684259935009198</v>
       </c>
       <c r="H97" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.11391288694833986</v>
       </c>
       <c r="I97" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>12.464513538056481</v>
       </c>
       <c r="J97" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>32.456082028628138</v>
       </c>
       <c r="K97" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>44.359223972630538</v>
+      </c>
+      <c r="L97" s="3">
+        <f t="shared" si="15"/>
         <v>18.647489328628183</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -4550,38 +4940,42 @@
         <v>17.670000000000002</v>
       </c>
       <c r="D98" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>312.96999799999998</v>
       </c>
       <c r="E98" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>290.81</v>
       </c>
       <c r="F98" s="1">
         <v>105</v>
       </c>
       <c r="G98" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>17.36384747</v>
       </c>
       <c r="H98" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.1654497787475169</v>
       </c>
       <c r="I98" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>12.627184452991299</v>
       </c>
       <c r="J98" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>33.045224807015678</v>
       </c>
       <c r="K98" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>45.034936044911682</v>
+      </c>
+      <c r="L98" s="3">
+        <f t="shared" si="15"/>
         <v>19.23663210701568</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -4592,38 +4986,42 @@
         <v>13.25</v>
       </c>
       <c r="D99" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>306.9099966</v>
       </c>
       <c r="E99" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>286.39</v>
       </c>
       <c r="F99" s="1">
         <v>113</v>
       </c>
       <c r="G99" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>13.072730249999999</v>
       </c>
       <c r="H99" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.21406226019508906</v>
       </c>
       <c r="I99" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>12.783465926539092</v>
       </c>
       <c r="J99" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>28.043632446133024</v>
       </c>
       <c r="K99" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>39.146017646556224</v>
+      </c>
+      <c r="L99" s="3">
+        <f t="shared" si="15"/>
         <v>14.235039746132998</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -4634,38 +5032,42 @@
         <v>17.309999999999999</v>
       </c>
       <c r="D100" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>315.7699973</v>
       </c>
       <c r="E100" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>290.45</v>
       </c>
       <c r="F100" s="1">
         <v>121</v>
       </c>
       <c r="G100" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>17.01434471</v>
       </c>
       <c r="H100" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.25892389338807958</v>
       </c>
       <c r="I100" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>12.930933836842986</v>
       </c>
       <c r="J100" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>33.731014659490874</v>
       </c>
       <c r="K100" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>47.430449838650475</v>
+      </c>
+      <c r="L100" s="3">
+        <f t="shared" si="15"/>
         <v>19.922421959490919</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -4676,38 +5078,42 @@
         <v>17.73</v>
       </c>
       <c r="D101" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>314.64999999999998</v>
       </c>
       <c r="E101" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>290.87</v>
       </c>
       <c r="F101" s="1">
         <v>129</v>
       </c>
       <c r="G101" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>17.42209793</v>
       </c>
       <c r="H101" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.2992316698461186</v>
       </c>
       <c r="I101" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>13.066744763521639</v>
       </c>
       <c r="J101" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>33.38329678780039</v>
       </c>
       <c r="K101" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>46.249513347800388</v>
+      </c>
+      <c r="L101" s="3">
+        <f t="shared" si="15"/>
         <v>19.574704087800399</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -4718,34 +5124,38 @@
         <v>16.670000000000002</v>
       </c>
       <c r="D102" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>315.6099974</v>
       </c>
       <c r="E102" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>289.81</v>
       </c>
       <c r="F102" s="1">
         <v>137</v>
       </c>
       <c r="G102" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>16.39300647</v>
       </c>
       <c r="H102" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0.33421939013812968</v>
       </c>
       <c r="I102" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>13.187667868532422</v>
       </c>
       <c r="J102" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>33.097164427819159</v>
       </c>
       <c r="K102" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
+        <v>47.05630462108396</v>
+      </c>
+      <c r="L102" s="3">
+        <f t="shared" si="15"/>
         <v>19.288571727819203</v>
       </c>
     </row>

</xml_diff>